<commit_message>
addtional methods for cell access. renaming artefacts
git-svn-id: https://svn.ecdf.ed.ac.uk/repo/biology/biodare@1247 b325261a-90cb-4c4b-9a13-2f556971fe3a
</commit_message>
<xml_diff>
--- a/src/test/resources/ed/synthsys/util/excel/SimpleImagingData.xlsx
+++ b/src/test/resources/ed/synthsys/util/excel/SimpleImagingData.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="315" windowWidth="24555" windowHeight="12780"/>
+    <workbookView xWindow="360" yWindow="315" windowWidth="24555" windowHeight="12780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Third" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Image Plane</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>second sheet</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -111,8 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,7 +423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -975,13 +979,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -994,6 +1001,14 @@
       </c>
       <c r="F3">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1">
+        <v>42248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>